<commit_message>
Excel files and TC dictionary file here
</commit_message>
<xml_diff>
--- a/NopCommerce/TestBase/TC_LoginTest_Report.xlsx
+++ b/NopCommerce/TestBase/TC_LoginTest_Report.xlsx
@@ -499,7 +499,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -564,26 +564,34 @@
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
+          <t>Valid Email &amp; Password</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>CorrectEmail@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>thatshouldmakeit</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>Navigate to Home page</t>
+        </is>
+      </c>
+      <c r="F2" s="7" t="inlineStr">
+        <is>
+          <t>Registration Successful and redirected to Login Page</t>
+        </is>
+      </c>
+      <c r="G2" s="7" t="inlineStr">
+        <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
-        <is>
-          <t>CorrectEmail@gmail.com</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>thatshouldmakeit</t>
-        </is>
-      </c>
-      <c r="E2" s="1" t="inlineStr">
-        <is>
-          <t>Navigate to Home page</t>
-        </is>
-      </c>
-      <c r="F2" s="7" t="n"/>
-      <c r="G2" s="7" t="n"/>
       <c r="H2" s="7" t="n"/>
     </row>
     <row r="3" ht="33.75" customHeight="1" thickBot="1">
@@ -594,26 +602,34 @@
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
+          <t>Invalid Password</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>CorrectEmail@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>thatshouldn't</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Login error: 'Wrong credentials'</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Failed to login</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
+        <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>CorrectEmail@gmail.com</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="inlineStr">
-        <is>
-          <t>thatshouldn't</t>
-        </is>
-      </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>Login error: 'Wrong credentials'</t>
-        </is>
-      </c>
-      <c r="F3" s="7" t="n"/>
-      <c r="G3" s="7" t="n"/>
       <c r="H3" s="7" t="n"/>
     </row>
     <row r="4" ht="33.75" customHeight="1" thickBot="1">
@@ -624,26 +640,34 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
+          <t>Invalid Email</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>NotcorrectEmail@gmail.com</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>thatshouldmakeit</t>
+        </is>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>Login error: 'No Customer account found'</t>
+        </is>
+      </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>Failed to login</t>
+        </is>
+      </c>
+      <c r="G4" s="7" t="inlineStr">
+        <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="C4" s="3" t="inlineStr">
-        <is>
-          <t>NotcorrectEmail@gmail.com</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="inlineStr">
-        <is>
-          <t>thatshouldmakeit</t>
-        </is>
-      </c>
-      <c r="E4" s="5" t="inlineStr">
-        <is>
-          <t>Login error: 'No Customer account found'</t>
-        </is>
-      </c>
-      <c r="F4" s="7" t="n"/>
-      <c r="G4" s="7" t="n"/>
       <c r="H4" s="7" t="n"/>
     </row>
     <row r="5" ht="33.75" customHeight="1"/>

</xml_diff>

<commit_message>
POM design pattern update
</commit_message>
<xml_diff>
--- a/NopCommerce/TestBase/TC_LoginTest_Report.xlsx
+++ b/NopCommerce/TestBase/TC_LoginTest_Report.xlsx
@@ -499,7 +499,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -584,7 +584,7 @@
       </c>
       <c r="F2" s="7" t="inlineStr">
         <is>
-          <t>Registration Successful and redirected to Login Page</t>
+          <t>Login Successful and redirected to Signed-in Page</t>
         </is>
       </c>
       <c r="G2" s="7" t="inlineStr">
@@ -658,16 +658,8 @@
           <t>Login error: 'No Customer account found'</t>
         </is>
       </c>
-      <c r="F4" s="7" t="inlineStr">
-        <is>
-          <t>Failed to login</t>
-        </is>
-      </c>
-      <c r="G4" s="7" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F4" s="7" t="n"/>
+      <c r="G4" s="7" t="n"/>
       <c r="H4" s="7" t="n"/>
     </row>
     <row r="5" ht="33.75" customHeight="1"/>

</xml_diff>